<commit_message>
atualizando requisitos funcionais e nao funcionais e atualizando a estrutura do README
</commit_message>
<xml_diff>
--- a/requisitos_e_curvas.xlsx
+++ b/requisitos_e_curvas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\IFSC\EMB\Sistemas-Embarcados\project\brewjoe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\IFSC\EMB\borrachoAPB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BD0572-8235-4DBE-B1E3-E2B473B1BAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BC40EC-BE4B-4FC3-8B5F-CA49120EE833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{61A80975-C060-4BB5-8D70-4F8BFC41141C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -157,202 +157,238 @@
     <t>Inserida via UART pelo usuário</t>
   </si>
   <si>
-    <t>O sistema deve controlar a temperatura com PID ou ON/OFF com histerese</t>
-  </si>
-  <si>
-    <t>Deve conter uma curva de temperatura padrão (67°C, 78°C, 100°C)</t>
-  </si>
-  <si>
-    <t>O sistema deve permitir entrada de novas curvas via comunicação serial</t>
-  </si>
-  <si>
-    <t>Mixer deve ser ativado se ΔT entre sensores &gt; 1°C</t>
-  </si>
-  <si>
-    <t>Sistema deve rodar em ESP32 e também ser simulável no PC</t>
-  </si>
-  <si>
-    <t>Código deve usar boas práticas em C++ com orientação a objetos</t>
-  </si>
-  <si>
-    <t>Projeto deve estar no GitHub, com versionamento contínuo</t>
-  </si>
-  <si>
-    <t>Deve ser usado Doxygen para gerar documentação automática</t>
-  </si>
-  <si>
-    <t>Interface serial precisa ser implementada</t>
-  </si>
-  <si>
-    <t>Necessário 2 sensores e lógica de comparação</t>
-  </si>
-  <si>
-    <t>Exige arquitetura com abstração/hardware</t>
-  </si>
-  <si>
-    <t>Uso de polimorfismo e métodos virtuais</t>
-  </si>
-  <si>
-    <t>A documentar progresso e commits</t>
-  </si>
-  <si>
-    <t>Documentação do projeto</t>
-  </si>
-  <si>
-    <t>Pode ser fixa no firmware, entrada customizada pelo usuário</t>
-  </si>
-  <si>
-    <t>Será validado com sensores reais assim que estiver completo</t>
-  </si>
-  <si>
     <t>Definição de Requisitos</t>
   </si>
   <si>
     <t>RF05</t>
   </si>
   <si>
-    <t>Exibição da temperatura atual e etapa atual em display LCD 16x4</t>
-  </si>
-  <si>
-    <t>Implementar driver do LCD e lógica para exibição dinâmica de dados</t>
-  </si>
-  <si>
     <t>RF06</t>
   </si>
   <si>
-    <t>Alertas visuais (LED) e sonoros (buzzer) para erros críticos</t>
-  </si>
-  <si>
-    <t>Adicionar circuito com LEDs e buzzer, implementar rotinas de alerta</t>
-  </si>
-  <si>
     <t>RF07</t>
   </si>
   <si>
     <t>RF08</t>
   </si>
   <si>
-    <t>Histórico dos últimos ciclos de fabricação</t>
-  </si>
-  <si>
-    <t>Armazenamento em memória não volátil (EEPROM/Flash) e rotina para leitura</t>
-  </si>
-  <si>
     <t>RF09</t>
   </si>
   <si>
-    <t>Detecção e alerta de perda de comunicação com sensores via I²C</t>
-  </si>
-  <si>
-    <t>Implementar monitoramento contínuo e rotinas de timeout e reconexão</t>
-  </si>
-  <si>
-    <t>Pausa e reinício das receitas em andamento</t>
-  </si>
-  <si>
-    <t>Criar mecanismo de pausa com salvamento de estado atual</t>
-  </si>
-  <si>
-    <t>Calibração dos sensores de temperatura</t>
-  </si>
-  <si>
-    <t>Desenvolver rotinas de calibração com entradas conhecidas (água gelada/quente)</t>
-  </si>
-  <si>
-    <t>Seleção entre controle PID ou ON/OFF ao iniciar operação</t>
-  </si>
-  <si>
-    <t>Criar rotina inicial que permita configuração via interface serial</t>
-  </si>
-  <si>
     <t>RNF05</t>
   </si>
   <si>
-    <t>Proteção elétrica contra curtos e sobreaquecimentos</t>
-  </si>
-  <si>
-    <t>Projeto do circuito com fusíveis, termistores e testes elétricos necessários</t>
-  </si>
-  <si>
     <t>RNF07</t>
   </si>
   <si>
     <t>RNF08</t>
   </si>
   <si>
-    <t>Produzir manual detalhado com fotos e diagramas de montagem</t>
-  </si>
-  <si>
     <t>RNF09</t>
   </si>
   <si>
-    <t>Logs detalhados para facilitar depuração e manutenção</t>
-  </si>
-  <si>
-    <t>Implementar módulo dedicado de logging via UART ou armazenamento local</t>
-  </si>
-  <si>
     <t>RNF10</t>
   </si>
   <si>
-    <t>Modularização do software para fácil expansão</t>
-  </si>
-  <si>
-    <t>Estruturação de código usando orientação a objetos com interfaces claras</t>
-  </si>
-  <si>
     <t>RNF11</t>
   </si>
   <si>
-    <t>Tempo de resposta máximo de 2 segundos na reação dos sensores/atuadores</t>
-  </si>
-  <si>
-    <t>Realizar medições e otimizações necessárias para garantir desempenho exigido</t>
-  </si>
-  <si>
     <t>RNF12</t>
   </si>
   <si>
-    <t>Implementação de testes unitários automatizados</t>
-  </si>
-  <si>
-    <t>Desenvolver testes usando frameworks como Unity ou GoogleTest</t>
-  </si>
-  <si>
     <t>RNF13</t>
   </si>
   <si>
     <t>RNF14</t>
   </si>
   <si>
-    <t>Implementação de funcionalidade adicional (alarme sonoro, visualização gráfica ou modo calibração)</t>
-  </si>
-  <si>
-    <t>Selecionar funcionalidade adicional, projetar e implementar completamente</t>
-  </si>
-  <si>
     <t>Baixa</t>
   </si>
   <si>
-    <t>Guia detalhado de como usar os módulos físicos do sistema</t>
-  </si>
-  <si>
-    <t>Ajuste manual da potência aplicada à resistência</t>
-  </si>
-  <si>
-    <t>Implementar entrada manual (GPIO ou serial) que consiga atuar em cima do controle automático</t>
-  </si>
-  <si>
-    <t>Implementar via UART a edição de curvas de usuário</t>
-  </si>
-  <si>
-    <t>Modificação de curvas via comunicação UART</t>
-  </si>
-  <si>
     <t>RNF15</t>
   </si>
   <si>
     <t>RNF16</t>
+  </si>
+  <si>
+    <t>O sistema deve aplicar algoritmos de controle (PID e/ou ON/OFF com histerese) para manter a temperatura do mosto dentro de uma margem de ±0.5∘C do setpoint definido pela curva de brassagem, acionando as resistências de aquecimento.</t>
+  </si>
+  <si>
+    <t>Especifica a precisão do controle. O PID é esperado para ser robusto.</t>
+  </si>
+  <si>
+    <t>O sistema deve carregar e executar uma curva de temperatura padrão pré-configurada (ex: 67°C por X min, 78°C por Y min, 100°C por Z min) ao iniciar a brassagem.</t>
+  </si>
+  <si>
+    <t>Deixa claro que a curva padrão é a default e como ela é iniciada.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir o upload de curvas de temperatura customizadas via interface serial (UART), ou via comandos em tela (KEYPAD 4X4). Cada curva deve conter múltiplos steps definidos por temperatura e duração, e o sistema deve validar a integridade dos dados recebidos.</t>
+  </si>
+  <si>
+    <t>Detalha a forma de upload e a necessidade de validação.</t>
+  </si>
+  <si>
+    <t>O sistema deve ativar automaticamente o mixer quando a diferença de temperatura entre quaisquer dois sensores exceder 1∘C (Delta T), com um retardo de ativação configurável, para garantir a homogeneização do mosto.</t>
+  </si>
+  <si>
+    <t>Necessário 2 sensores (TEMPERATURA) em dois extremos da bacia e lógica de comparação, da mesma forma um dispositivo com motor de rotação par ao MIXER.</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir continuamente no display OLED (ou LCD) a temperatura atual do mosto (obtida pelo sensor principal), o setpoint da etapa atual da curva, o tempo restante para a etapa atual e o status operacional do mixer e resistências.</t>
+  </si>
+  <si>
+    <t>Especifica quais informações devem ser mostradas e de qual sensor. Detalha o "estado atual".</t>
+  </si>
+  <si>
+    <t>O sistema deve emitir alertas visuais (LEDs) ou sonoros (BUZZER) para notificar o usuário sobre erros críticos de operação (ex: falha de sensor, sobreaquecimento, erro de comunicação), indicando o tipo de falha.</t>
+  </si>
+  <si>
+    <t>Especifica os tipos de alerta e a informação a ser passada (tipo de falha).</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir ao usuário selecionar o modo de controle (PID ou ON/OFF) antes ou durante o início de uma nova brassagem, através da interface de usuário (teclado ou serial).</t>
+  </si>
+  <si>
+    <t>Define quando a seleção pode ocorrer e por qual interface.</t>
+  </si>
+  <si>
+    <t>O sistema deve implementar um "Modo de Calibração" para os sensores de temperatura, permitindo ao usuário ajustar offsets ou fatores de calibração para leituras mais precisas, com base em temperaturas de referência conhecidas.</t>
+  </si>
+  <si>
+    <t>Funcionalidade adicional interessante.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir ao usuário visualizar e modificar parâmetros específicos da curva de brassagem em tempo real (ex: setpoint de temperatura, duração da etapa) através da comunicação UART, sem interromper o processo atual.</t>
+  </si>
+  <si>
+    <t>Detalha a modificação de curvas durante a operação, um requisito mais avançado que "modificação de curvas".</t>
+  </si>
+  <si>
+    <t>O sistema deve registrar em memória não volátil (Flash ou EEPROM) os parâmetros de cada brassagem concluída (curva utilizada, temperaturas máximas/mínimas atingidas, duração total) e permitir a consulta desses logs via UART.</t>
+  </si>
+  <si>
+    <t>Funcionalidade adicional de histórico, útil para otimização de receitas.</t>
+  </si>
+  <si>
+    <t>RF10</t>
+  </si>
+  <si>
+    <t>A arquitetura de software deve ser portável, permitindo que o sistema seja executado tanto em uma plataforma embarcada (ESP32) quanto em um ambiente de simulação no PC, utilizando abstração de hardware (HAL) para facilitar a troca de implementações de periféricos.</t>
+  </si>
+  <si>
+    <t>Enfatiza a portabilidade e o uso de HAL para atingir esse objetivo.</t>
+  </si>
+  <si>
+    <t>O código-fonte deve ser implementado em C++ seguindo princípios de Orientação a Objetos (OO), com uso extensivo de polimorfismo e métodos virtuais, para garantir modularidade, reusabilidade e extensibilidade do sistema.</t>
+  </si>
+  <si>
+    <t>Aprofunda em "boas práticas" especificando OO, polimorfismo e métodos virtuais, o que é fundamental para a simulação no PC.</t>
+  </si>
+  <si>
+    <t>O projeto deve ser versionado no GitHub com um histórico de commits claro e descritivo, refletindo o progresso incremental e as mudanças significativas em cada funcionalidade implementada.</t>
+  </si>
+  <si>
+    <t>Adiciona "histórico de commits claro e descritivo" para enfatizar a qualidade do versionamento.</t>
+  </si>
+  <si>
+    <t>Toda a base de código deve ser documentada utilizando Doxygen, gerando uma documentação técnica completa das funções, classes, variáveis e módulos, facilitando a compreensão e manutenção por outros desenvolvedores.</t>
+  </si>
+  <si>
+    <t>Especifica "toda a base de código" e o benefício da documentação.</t>
+  </si>
+  <si>
+    <t>O sistema deve incorporar proteção elétrica robusta contra curtos-circuitos, sobreaquecimento e surtos de tensão nos circuitos de controle das resistências e do mixer, garantindo a segurança do equipamento e do usuário.</t>
+  </si>
+  <si>
+    <t>Projeto do circuito com fusíveis, termistores e testes elétricos necessários.</t>
+  </si>
+  <si>
+    <t>Deve ser fornecido um manual de montagem detalhado, com diagramas de fiação, fotos ilustrativas e lista de materiais (BOM), para permitir que um usuário replique o hardware do sistema.</t>
+  </si>
+  <si>
+    <t>Produzir manual detalhado com fotos e diagramas de montagem.</t>
+  </si>
+  <si>
+    <t>O sistema deve gerar logs de eventos detalhados (ex: mudanças de setpoint, ativação/desativação de atuadores, erros de sensor) via UART, que possam ser facilmente consumidos e analisados por uma aplicação no PC para depuração e monitoramento.</t>
+  </si>
+  <si>
+    <t>Implementar módulo dedicado de logging via UART ou armazenamento local.</t>
+  </si>
+  <si>
+    <t>O software deve ser projetado com alta coesão e baixo acoplamento entre os módulos, utilizando interfaces bem definidas para facilitar futuras expansões e manutenções sem impacto em outras partes do sistema.</t>
+  </si>
+  <si>
+    <t>O sistema deve reagir a alterações nos sensores ou comandos de controle e atualizar o estado dos atuadores e do display em no máximo 500ms, para garantir uma experiência de usuário responsiva e controle em tempo real.</t>
+  </si>
+  <si>
+    <t>Especifica um tempo de resposta (ex: 500ms) para tornar o requisito mensurável e mais exigente que 2s, dado o FreeRTOS.</t>
+  </si>
+  <si>
+    <t>Estruturação de código usando orientação a objetos com interfaces claras.</t>
+  </si>
+  <si>
+    <t>O software deve ser submetido a testes unitários automatizados para as camadas de lógica de controle e módulos críticos, utilizando um framework de teste (ex: Unity, Google Test) para garantir a robustez e correção do código.</t>
+  </si>
+  <si>
+    <t>Desenvolver testes usando frameworks como Unity ou GoogleTest.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir o ajuste manual da potência de saída para as resistências (ex: via PWM), permitindo ao usuário sobrescrever temporariamente o controle automático em situações específicas de fine-tuning ou emergência.</t>
+  </si>
+  <si>
+    <t>Implementar entrada manual (GPIO ou serial) que consiga atuar em cima do controle automático.</t>
+  </si>
+  <si>
+    <t>O sistema deve detectar e alertar sobre a perda de comunicação com qualquer sensor I²C (ex: por timeout ou falha de CRC), e tentar restabelecer a comunicação automaticamente antes de reportar uma falha crítica.</t>
+  </si>
+  <si>
+    <t>Detalha a detecção da perda de comunicação e a tentativa de recuperação.</t>
+  </si>
+  <si>
+    <t>O sistema deve ser capaz de calibrar automaticamente ou semi-automaticamente os sensores de temperatura durante o processo de brassagem, compensando variações devido à imersão ou tipo de sensor, utilizando pontos de calibração conhecidos.</t>
+  </si>
+  <si>
+    <t>Melhora e detalha a calibração, tornando-a mais avançada.</t>
+  </si>
+  <si>
+    <t>A interface de usuário via teclado deve ser intuitiva e eficiente, permitindo a navegação pelos menus e a entrada de dados com um mínimo de passos, para uma boa experiência do usuário.</t>
+  </si>
+  <si>
+    <t>Requisito de usabilidade importante, especialmente para interfaces embarcadas.</t>
+  </si>
+  <si>
+    <t>O consumo de energia do sistema deve ser otimizado para operação de longo prazo, especialmente em modos de espera ou monitoramento, para minimizar o aquecimento desnecessário e potencializar o uso de fontes de energia.</t>
+  </si>
+  <si>
+    <t>Requisito de eficiência e sustentabilidade.</t>
+  </si>
+  <si>
+    <t>RNF17</t>
+  </si>
+  <si>
+    <t>O código deve seguir um guia de estilo de codificação (ex: Google Style Guide, MISRA C/C++) para garantir consistência, legibilidade e manutenibilidade em todo o projeto.</t>
+  </si>
+  <si>
+    <t>Requisito de qualidade de código mais formal.</t>
+  </si>
+  <si>
+    <t>RF11</t>
+  </si>
+  <si>
+    <t>O sistema deve suportar a criação de "receitas", que são sequências pré-definidas de curvas de brassagem (ex: Mash, Boil, Fermentação), permitindo ao usuário selecionar e executar uma receita completa.</t>
+  </si>
+  <si>
+    <t>Eleva o projeto de controle de uma única curva para o gerenciamento de múltiplos estágios da produção de cerveja.</t>
+  </si>
+  <si>
+    <t>RF12</t>
+  </si>
+  <si>
+    <t>O sistema deve fornecer feedback visual (ex: ícones no display ou LEDs de status) sobre o estado atual dos atuadores (resistências ligadas/desligadas, mixer ativo/inativo), mesmo quando não houver erro crítico, para facilitar o monitoramento do processo.</t>
+  </si>
+  <si>
+    <t>Melhora a usabilidade e a visualização do estado do sistema em tempo real.</t>
   </si>
 </sst>
 </file>
@@ -784,17 +820,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C660D932-BB33-4FA6-8C95-0F54D723694B}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="3" max="3" width="92" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -804,7 +840,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -830,7 +866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -838,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -850,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -861,7 +897,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
@@ -873,10 +909,10 @@
         <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -884,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
@@ -896,10 +932,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -907,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -919,18 +955,18 @@
         <v>11</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -942,21 +978,21 @@
         <v>11</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -965,18 +1001,18 @@
         <v>20</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -988,21 +1024,21 @@
         <v>11</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -1011,21 +1047,21 @@
         <v>20</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -1034,156 +1070,156 @@
         <v>11</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>9</v>
@@ -1195,35 +1231,35 @@
         <v>20</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
@@ -1232,30 +1268,30 @@
         <v>90</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>16</v>
@@ -1264,21 +1300,21 @@
         <v>20</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1287,207 +1323,299 @@
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="7" t="s">
+      <c r="E28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="G28" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="36" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B37" s="2">
         <v>0</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C37" s="2">
         <v>67</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E37" s="2">
         <v>78</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F37" s="2">
         <v>20</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G37" s="2">
         <v>100</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B38" s="2">
         <v>0</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C38" s="2">
         <v>65</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D38" s="2">
         <v>15</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E38" s="2">
         <v>72</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F38" s="2">
         <v>30</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G38" s="2">
         <v>98</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>